<commit_message>
removed lte antenna from bom
</commit_message>
<xml_diff>
--- a/hardware/permamote_lte/rev_a/permamote-lte_bom.xlsx
+++ b/hardware/permamote_lte/rev_a/permamote-lte_bom.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="permamote_lte" localSheetId="0">Sheet1!$A$1:$S$53</definedName>
+    <definedName name="permamote_lte" localSheetId="0">Sheet1!$A$1:$S$52</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="293">
   <si>
     <t>Qty</t>
   </si>
@@ -114,24 +114,6 @@
   </si>
   <si>
     <t>VENDOR</t>
-  </si>
-  <si>
-    <t>FXUB65.07.0180C</t>
-  </si>
-  <si>
-    <t>ANT2</t>
-  </si>
-  <si>
-    <t>RF ANT 829MHZ/2.2GHZ FLAT PATCH</t>
-  </si>
-  <si>
-    <t>931-1455-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/taoglas-limited/FXUB65.07.0180C/931-1455-ND/6362793</t>
-  </si>
-  <si>
-    <t>Taoglas Limited</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -1276,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L23" workbookViewId="0">
-      <selection activeCell="T58" sqref="T58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,61 +1342,57 @@
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
@@ -1441,7 +1419,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
@@ -1450,19 +1428,19 @@
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1470,37 +1448,41 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1513,138 +1495,134 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1665,100 +1643,100 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1462350001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1462350001</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>67</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q10" s="1"/>
+      <c r="O10" s="1">
+        <v>1462350001</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1462350001</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1462350001</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1462350001</v>
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="1">
-        <v>1462350001</v>
-      </c>
-      <c r="P11" s="1">
-        <v>1462350001</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>78</v>
@@ -1772,7 +1750,9 @@
       <c r="J12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1793,30 +1773,28 @@
       <c r="C13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1">
+        <v>74437324220</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1" t="s">
-        <v>86</v>
+      <c r="P13" s="1">
+        <v>74437324220</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1826,33 +1804,35 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D14" s="1">
-        <v>74437324220</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1">
-        <v>74437324220</v>
+        <v>3039</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1865,32 +1845,30 @@
         <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1">
-        <v>3039</v>
+      <c r="P15" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -1900,19 +1878,19 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>98</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1933,28 +1911,28 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1962,111 +1940,111 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="K18" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>470</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1">
-        <v>470</v>
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2074,7 +2052,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -2084,16 +2062,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>28</v>
@@ -2102,7 +2080,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2110,7 +2088,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -2120,25 +2098,25 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2146,7 +2124,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -2156,25 +2134,25 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2182,7 +2160,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -2192,25 +2170,25 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2218,7 +2196,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2228,25 +2206,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2254,7 +2232,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -2264,25 +2242,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2290,7 +2268,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -2300,25 +2278,25 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -2326,7 +2304,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -2336,19 +2314,19 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2356,13 +2334,15 @@
       <c r="J28" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -2400,7 +2380,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -2410,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>157</v>
@@ -2438,7 +2418,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
@@ -2448,10 +2428,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>163</v>
@@ -2460,23 +2440,23 @@
         <v>164</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K31" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -2498,23 +2478,23 @@
         <v>170</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>177</v>
+        <v>289</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -2524,10 +2504,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>175</v>
@@ -2536,101 +2516,101 @@
         <v>176</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="G33" s="1"/>
+        <v>177</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>181</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>181</v>
+        <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>182</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>184</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="1" t="s">
-        <v>181</v>
-      </c>
+      <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
+      <c r="S34" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>25</v>
+        <v>183</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>26</v>
+        <v>184</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+      <c r="P35" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
-      <c r="S35" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2662,10 +2642,12 @@
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
+      <c r="N36" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -2675,108 +2657,106 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1020</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F37" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>200</v>
-      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="N37" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
+      <c r="S37" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1020</v>
+        <v>199</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>201</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
+      <c r="P38" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -2786,35 +2766,35 @@
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
@@ -2824,35 +2804,35 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="1" t="s">
-        <v>225</v>
+      <c r="P41" s="1">
+        <v>693043020611</v>
       </c>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2868,42 +2848,42 @@
         <v>226</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
-      <c r="P42" s="1">
-        <v>693043020611</v>
+      <c r="P42" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>232</v>
@@ -2912,61 +2892,61 @@
         <v>233</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>296</v>
+        <v>234</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="K44" s="1" t="s">
         <v>242</v>
       </c>
+      <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="N44" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -2976,35 +2956,37 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G45" s="1"/>
+        <v>248</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="K45" s="1"/>
+        <v>250</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
-      <c r="N45" s="1" t="s">
-        <v>249</v>
-      </c>
+      <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -3014,37 +2996,35 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>255</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -3074,15 +3054,13 @@
       <c r="J47" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
@@ -3103,23 +3081,17 @@
       <c r="E48" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1" t="s">
-        <v>269</v>
-      </c>
+      <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="1" t="s">
-        <v>270</v>
-      </c>
+      <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
@@ -3128,34 +3100,40 @@
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
+      <c r="J49" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
+      <c r="P49" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>274</v>
@@ -3169,77 +3147,81 @@
       <c r="E50" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>277</v>
-      </c>
+      <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="1" t="s">
-        <v>278</v>
-      </c>
+      <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-      <c r="P50" s="1" t="s">
-        <v>279</v>
-      </c>
+      <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
+      <c r="S50" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>279</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
+      <c r="J51" s="1" t="s">
+        <v>280</v>
+      </c>
       <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
+      <c r="L51" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+      <c r="P51" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-      <c r="S51" t="s">
-        <v>187</v>
+      <c r="R51" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -3247,58 +3229,18 @@
       <c r="J52" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1" t="s">
-        <v>283</v>
-      </c>
+      <c r="K52" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="Q52" s="1"/>
-      <c r="R52" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>2</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
+      <c r="R52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove tp and jlink from bom
</commit_message>
<xml_diff>
--- a/hardware/permamote_lte/rev_a/permamote-lte_bom.xlsx
+++ b/hardware/permamote_lte/rev_a/permamote-lte_bom.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="permamote_lte_1" localSheetId="0">Sheet1!$A$1:$S$52</definedName>
+    <definedName name="permamote_lte" localSheetId="0">Sheet1!$A$1:$S$48</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="275">
   <si>
     <t>Qty</t>
   </si>
@@ -197,18 +197,12 @@
     <t>10k</t>
   </si>
   <si>
-    <t>R5, R6, R7, R8, R9, R10</t>
-  </si>
-  <si>
     <t xml:space="preserve">311-10KJRCT-ND </t>
   </si>
   <si>
     <t>RC0402JR-0710KL</t>
   </si>
   <si>
-    <t>R11, R12, R13</t>
-  </si>
-  <si>
     <t>10nF</t>
   </si>
   <si>
@@ -353,18 +347,12 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>C11, C12, C13, C14, C15</t>
-  </si>
-  <si>
     <t>445-5947-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">C1005X5R0J475K050BC </t>
   </si>
   <si>
-    <t>C16</t>
-  </si>
-  <si>
     <t>R1, R2, R3</t>
   </si>
   <si>
@@ -698,9 +686,6 @@
     <t>WURTH_NANO_SIM</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
     <t>WURTH Nano SIM Connector</t>
   </si>
   <si>
@@ -824,12 +809,6 @@
     <t>AM-1454CA</t>
   </si>
   <si>
-    <t>TC2030-JLINK-NL</t>
-  </si>
-  <si>
-    <t>TC2030-IDC-NL</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -851,12 +830,6 @@
     <t>TCS34725FN</t>
   </si>
   <si>
-    <t>TEST-POINT</t>
-  </si>
-  <si>
-    <t>PAD.03X.03</t>
-  </si>
-  <si>
     <t>TPD3F303DPVR</t>
   </si>
   <si>
@@ -899,9 +872,6 @@
     <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29</t>
-  </si>
-  <si>
     <t>J4, J5</t>
   </si>
   <si>
@@ -911,10 +881,10 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>311-10KJRCT-ND</t>
-  </si>
-  <si>
-    <t>C1005X5R0J475K050BC</t>
+    <t>R5, R6, R7, R8, R9, R10, R11, R12, R13</t>
+  </si>
+  <si>
+    <t>C11, C12, C13, C14, C15, C16</t>
   </si>
 </sst>
 </file>
@@ -968,7 +938,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="permamote-lte_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="permamote-lte" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1234,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="91" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,7 +1288,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1471,7 +1441,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>44</v>
@@ -1483,7 +1453,7 @@
         <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>35</v>
@@ -1492,7 +1462,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1500,35 +1470,35 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>283</v>
+        <v>49</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1536,26 +1506,26 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>22</v>
@@ -1564,7 +1534,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1572,127 +1542,129 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1462350001</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1462350001</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="J9" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q9" s="1"/>
+      <c r="O9" s="1">
+        <v>1462350001</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1462350001</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1462350001</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1462350001</v>
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="1">
-        <v>1462350001</v>
-      </c>
-      <c r="P10" s="1">
-        <v>1462350001</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K11" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1702,16 +1674,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="D12" s="1">
+        <v>74437324220</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>28</v>
@@ -1720,17 +1692,15 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="1" t="s">
-        <v>76</v>
+      <c r="P12" s="1">
+        <v>74437324220</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1740,33 +1710,35 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="1">
-        <v>74437324220</v>
+        <v>79</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1">
-        <v>74437324220</v>
+        <v>3039</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1776,35 +1748,33 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>281</v>
+        <v>85</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1">
-        <v>3039</v>
+      <c r="P14" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1814,16 +1784,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>35</v>
@@ -1832,7 +1802,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1840,35 +1810,35 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>93</v>
+        <v>274</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1876,29 +1846,29 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>470</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1917,12 +1887,12 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>19</v>
@@ -1931,7 +1901,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>22</v>
@@ -1940,7 +1910,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1948,35 +1918,35 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1" t="s">
-        <v>284</v>
+        <v>103</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1">
-        <v>470</v>
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1984,35 +1954,35 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2020,35 +1990,35 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2056,17 +2026,17 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -2075,7 +2045,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>35</v>
@@ -2084,7 +2054,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2092,35 +2062,35 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2128,26 +2098,26 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>35</v>
@@ -2156,7 +2126,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2164,35 +2134,35 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2200,420 +2170,419 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K26" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>133</v>
+        <v>267</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K27" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+        <v>249</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>159</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>162</v>
+        <v>22</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>164</v>
-      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1" t="s">
-        <v>165</v>
-      </c>
+      <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
+      <c r="S32" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>256</v>
+        <v>151</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
+      <c r="N34" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="P34" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
-      <c r="S34" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>174</v>
+        <v>183</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1020</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>176</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>178</v>
-      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="1" t="s">
-        <v>173</v>
-      </c>
+      <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
+      <c r="S35" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="1" t="s">
-        <v>185</v>
-      </c>
+      <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -2623,68 +2592,73 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1020</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="J37" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+      <c r="P37" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
@@ -2694,35 +2668,35 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>191</v>
+        <v>268</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="1" t="s">
-        <v>202</v>
+      <c r="P39" s="1">
+        <v>693043020611</v>
       </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -2732,73 +2706,71 @@
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>206</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="1">
-        <v>693043020611</v>
+      <c r="P41" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2808,71 +2780,75 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>219</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="N42" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>278</v>
+        <v>224</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G43" s="1"/>
+        <v>232</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -2882,35 +2858,35 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="K44" s="1"/>
+        <v>241</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
-      <c r="N44" s="1" t="s">
-        <v>232</v>
-      </c>
+      <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -2920,75 +2896,72 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>238</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>240</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
+      <c r="S45" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>247</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -2998,119 +2971,103 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>251</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
+      <c r="L47" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
+      <c r="R47" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F48" s="1"/>
+        <v>270</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
+      <c r="J48" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
+      <c r="P48" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>1</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>260</v>
-      </c>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="1" t="s">
-        <v>261</v>
-      </c>
+      <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="1" t="s">
-        <v>262</v>
-      </c>
+      <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>29</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>279</v>
-      </c>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -3124,85 +3081,6 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
-      <c r="S50" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>1</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>2</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>